<commit_message>
Nuevas Funcionalidades en el Backend
</commit_message>
<xml_diff>
--- a/Documentacion/Product backlog/Product Backlog v1.2/Historias de Usuario versión 1.2.xlsx
+++ b/Documentacion/Product backlog/Product Backlog v1.2/Historias de Usuario versión 1.2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsaet\OneDrive\Escritorio\Proyecto_E-commerce\Documentacion\Product backlog\Product Backlog v1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350354C-256C-4C2F-BFCB-3AA280243098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B29C95-A755-4B66-BEFC-D5FAB8B61FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -482,7 +482,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +507,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -839,7 +845,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -892,18 +898,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -913,21 +907,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -936,9 +915,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -948,6 +924,63 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,8 +1288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1DBEB7-C3D2-4473-9B85-4CF26F3AA489}">
   <dimension ref="B1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,324 +1308,324 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="2:9" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="H4" s="32" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="30"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="2:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="42" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="19" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="45" t="s">
         <v>87</v>
       </c>
       <c r="I7" s="6"/>
     </row>
     <row r="8" spans="2:9" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="20" t="s">
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48" t="s">
         <v>88</v>
       </c>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="42" t="s">
         <v>89</v>
       </c>
       <c r="I9" s="6"/>
     </row>
     <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="19" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="45" t="s">
         <v>90</v>
       </c>
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35" t="s">
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51" t="s">
         <v>91</v>
       </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="42" t="s">
         <v>92</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="19" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="45" t="s">
         <v>93</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="27"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="20" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="48" t="s">
         <v>94</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="42" t="s">
         <v>95</v>
       </c>
       <c r="I15" s="6"/>
     </row>
     <row r="16" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="19" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="45" t="s">
         <v>96</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="27"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="20" t="s">
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="48" t="s">
         <v>97</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="42" t="s">
         <v>98</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="19" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="45" t="s">
         <v>99</v>
       </c>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35" t="s">
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="51" t="s">
         <v>100</v>
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+    <row r="21" spans="2:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="37" t="s">
         <v>32</v>
       </c>
       <c r="H21" s="23" t="s">
@@ -1600,35 +1633,35 @@
       </c>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="27"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+    <row r="22" spans="2:9" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="36"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
       <c r="H22" s="20" t="s">
         <v>102</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="37" t="s">
         <v>61</v>
       </c>
       <c r="H23" s="23" t="s">
@@ -1637,34 +1670,34 @@
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="27"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
       <c r="H24" s="20" t="s">
         <v>104</v>
       </c>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="37" t="s">
         <v>72</v>
       </c>
       <c r="H25" s="23" t="s">
@@ -1673,46 +1706,46 @@
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="26"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
       <c r="H26" s="19" t="s">
         <v>106</v>
       </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="27"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
       <c r="H27" s="20" t="s">
         <v>107</v>
       </c>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="32" t="s">
+      <c r="F28" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="37" t="s">
         <v>66</v>
       </c>
       <c r="H28" s="23" t="s">
@@ -1721,34 +1754,34 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="27"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
       <c r="H29" s="20" t="s">
         <v>109</v>
       </c>
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="32" t="s">
+      <c r="C30" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="32" t="s">
+      <c r="E30" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="37" t="s">
         <v>69</v>
       </c>
       <c r="H30" s="23" t="s">
@@ -1757,34 +1790,34 @@
       <c r="I30" s="6"/>
     </row>
     <row r="31" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="27"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
       <c r="H31" s="20" t="s">
         <v>111</v>
       </c>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E32" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="32" t="s">
+      <c r="G32" s="37" t="s">
         <v>75</v>
       </c>
       <c r="H32" s="23" t="s">
@@ -1793,34 +1826,34 @@
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="27"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
       <c r="H33" s="20" t="s">
         <v>113</v>
       </c>
       <c r="I33" s="6"/>
     </row>
     <row r="34" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="32" t="s">
+      <c r="E34" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="32" t="s">
+      <c r="G34" s="37" t="s">
         <v>78</v>
       </c>
       <c r="H34" s="23" t="s">
@@ -1829,34 +1862,34 @@
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="2:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="27"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
       <c r="H35" s="20" t="s">
         <v>115</v>
       </c>
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D36" s="32" t="s">
+      <c r="D36" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="32" t="s">
+      <c r="E36" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="32" t="s">
+      <c r="G36" s="37" t="s">
         <v>31</v>
       </c>
       <c r="H36" s="23" t="s">
@@ -1865,58 +1898,58 @@
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="27"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
       <c r="H37" s="20" t="s">
         <v>117</v>
       </c>
       <c r="I37" s="8"/>
     </row>
     <row r="38" spans="2:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="37" t="s">
+      <c r="E38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="F38" s="37" t="s">
+      <c r="F38" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="G38" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="H38" s="38" t="s">
+      <c r="H38" s="29" t="s">
         <v>118</v>
       </c>
       <c r="I38" s="8"/>
     </row>
     <row r="39" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="32" t="s">
+      <c r="E39" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="32" t="s">
+      <c r="G39" s="37" t="s">
         <v>85</v>
       </c>
       <c r="H39" s="23" t="s">
@@ -1925,12 +1958,12 @@
       <c r="I39" s="8"/>
     </row>
     <row r="40" spans="2:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="27"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
       <c r="H40" s="20" t="s">
         <v>120</v>
       </c>
@@ -2373,13 +2406,72 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="B1:H3"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="C12:C14"/>
@@ -2392,72 +2484,13 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="B1:H3"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="70" orientation="landscape" r:id="rId1"/>

</xml_diff>